<commit_message>
done 3. Create new transaction - Withdrawals
</commit_message>
<xml_diff>
--- a/Data Sources/test_data.xlsx
+++ b/Data Sources/test_data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Thuan\Desktop\software_testing_katalon\Data Sources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Thuan\Desktop\Workspace\software_testing_katalon\Data Sources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F4D8ECC-A182-4FE0-AB1E-59FE7BE12519}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7064048F-388C-4B85-A279-FAA38E993B8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="3" activeTab="6" xr2:uid="{E92A2BA7-7C6F-4CAA-BFF3-4F484A7C023D}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="5" activeTab="9" xr2:uid="{E92A2BA7-7C6F-4CAA-BFF3-4F484A7C023D}"/>
   </bookViews>
   <sheets>
     <sheet name="new_asset_sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,9 @@
     <sheet name="new_expense_sheet1" sheetId="6" r:id="rId5"/>
     <sheet name="new_expense_sheet2" sheetId="7" r:id="rId6"/>
     <sheet name="new_expense_sheet3" sheetId="9" r:id="rId7"/>
-    <sheet name="withdrawals_sheet1" sheetId="8" r:id="rId8"/>
+    <sheet name="withdrawals_sheet1" sheetId="10" r:id="rId8"/>
+    <sheet name="withdrawals_sheet2" sheetId="11" r:id="rId9"/>
+    <sheet name="withdrawals_sheet3" sheetId="12" r:id="rId10"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -32,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="92">
   <si>
     <t>Name</t>
   </si>
@@ -178,79 +180,136 @@
     <t>DE23100000001234567890</t>
   </si>
   <si>
+    <t>Euro (€)</t>
+  </si>
+  <si>
+    <t>British Pound (£)</t>
+  </si>
+  <si>
+    <t>Hungarian forint (Ft)</t>
+  </si>
+  <si>
+    <t>US Dollar ($)</t>
+  </si>
+  <si>
+    <t>12/31/2023</t>
+  </si>
+  <si>
+    <t>file</t>
+  </si>
+  <si>
+    <t>C:\Users\Thuan\Desktop\software_testing_katalon\Data Sources\attachment_file_gt2mb.pdf</t>
+  </si>
+  <si>
+    <t>C:\Users\Thuan\Desktop\software_testing_katalon\Data Sources\attachment_file_lt2mb.pdf</t>
+  </si>
+  <si>
+    <t>413 Request Entity Too Large</t>
+  </si>
+  <si>
+    <t>expected_message</t>
+  </si>
+  <si>
+    <t>test 20</t>
+  </si>
+  <si>
+    <t>test 21</t>
+  </si>
+  <si>
+    <t>Success! New account "test 20" stored!</t>
+  </si>
+  <si>
+    <t>account_name</t>
+  </si>
+  <si>
+    <t>expected_value</t>
+  </si>
+  <si>
+    <t>The house</t>
+  </si>
+  <si>
+    <t>dropdown open</t>
+  </si>
+  <si>
+    <t>asdsadasdsadasdasdcasdasd</t>
+  </si>
+  <si>
+    <t>dropdown</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>source_account</t>
+  </si>
+  <si>
     <t>description</t>
   </si>
   <si>
-    <t>source</t>
-  </si>
-  <si>
-    <t>amount</t>
-  </si>
-  <si>
-    <t>destination</t>
-  </si>
-  <si>
-    <t>foreign_amount</t>
+    <t>destination_account</t>
+  </si>
+  <si>
+    <t>ammount</t>
+  </si>
+  <si>
+    <t>foreign_account</t>
+  </si>
+  <si>
+    <t>testcase</t>
+  </si>
+  <si>
+    <t>AMEX Credit Card debt</t>
+  </si>
+  <si>
+    <t>TC_3.6</t>
+  </si>
+  <si>
+    <t>TC_3.7</t>
   </si>
   <si>
     <t>The transaction amount must be greater than 0.</t>
   </si>
   <si>
-    <t>Source and destination are the same.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">test </t>
-  </si>
-  <si>
-    <t>There was something wrong with your submission. Please check out the errors.</t>
-  </si>
-  <si>
-    <t>Success! Successfully created new transaction "test"</t>
-  </si>
-  <si>
-    <t>The transaction amount field is required.</t>
-  </si>
-  <si>
-    <t>Australian dollar (A$)</t>
-  </si>
-  <si>
-    <t>Euro (€)</t>
-  </si>
-  <si>
-    <t>British Pound (£)</t>
-  </si>
-  <si>
-    <t>Hungarian forint (Ft)</t>
-  </si>
-  <si>
-    <t>US Dollar ($)</t>
-  </si>
-  <si>
-    <t>12/31/2023</t>
-  </si>
-  <si>
-    <t>file</t>
-  </si>
-  <si>
-    <t>C:\Users\Thuan\Desktop\software_testing_katalon\Data Sources\attachment_file_gt2mb.pdf</t>
-  </si>
-  <si>
-    <t>C:\Users\Thuan\Desktop\software_testing_katalon\Data Sources\attachment_file_lt2mb.pdf</t>
-  </si>
-  <si>
-    <t>413 Request Entity Too Large</t>
-  </si>
-  <si>
-    <t>expected_message</t>
-  </si>
-  <si>
-    <t>test 20</t>
-  </si>
-  <si>
-    <t>test 21</t>
-  </si>
-  <si>
-    <t>Success! New account "test 20" stored!</t>
+    <t>Success! Successfully created new transaction "([a-zA-Z]+)"</t>
+  </si>
+  <si>
+    <t>TC_3.12</t>
+  </si>
+  <si>
+    <t>Error! There was something wrong with your submission. Please check out the errors.</t>
+  </si>
+  <si>
+    <t>TC_3.13</t>
+  </si>
+  <si>
+    <t>TC_3.16</t>
+  </si>
+  <si>
+    <t>month</t>
+  </si>
+  <si>
+    <t>day</t>
+  </si>
+  <si>
+    <t>year</t>
+  </si>
+  <si>
+    <t>hour</t>
+  </si>
+  <si>
+    <t>minute</t>
+  </si>
+  <si>
+    <t>07</t>
+  </si>
+  <si>
+    <t>15</t>
+  </si>
+  <si>
+    <t>2023-12-15T16:20</t>
+  </si>
+  <si>
+    <t>2024-11-26T07:15</t>
   </si>
 </sst>
 </file>
@@ -260,7 +319,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
   </numFmts>
-  <fonts count="16">
+  <fonts count="15">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -292,14 +351,6 @@
       <family val="1"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="8"/>
       <name val="Arial"/>
       <family val="2"/>
@@ -328,17 +379,6 @@
       <family val="2"/>
     </font>
     <font>
-      <sz val="11"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="12"/>
       <name val="Arial"/>
       <family val="2"/>
@@ -354,6 +394,20 @@
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF051B52"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF333333"/>
       <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -376,11 +430,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -400,39 +453,44 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+      <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="1">
     <cellStyle name="Bình thường" xfId="0" builtinId="0"/>
-    <cellStyle name="Siêu kết nối" xfId="1" builtinId="8"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -747,7 +805,7 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D4" sqref="A1:XFD1048576"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.09765625" defaultRowHeight="13.8"/>
@@ -799,67 +857,140 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1DBF8AA0-9DC2-4135-9B59-F025B517EDDD}">
+  <dimension ref="A1:F3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K6" sqref="K6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8"/>
+  <cols>
+    <col min="6" max="6" width="15.69921875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B1" t="s">
+        <v>83</v>
+      </c>
+      <c r="C1" t="s">
+        <v>85</v>
+      </c>
+      <c r="D1" t="s">
+        <v>86</v>
+      </c>
+      <c r="E1" t="s">
+        <v>87</v>
+      </c>
+      <c r="F1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" s="25">
+        <v>15</v>
+      </c>
+      <c r="B2" s="25">
+        <v>12</v>
+      </c>
+      <c r="C2" s="25">
+        <v>2023</v>
+      </c>
+      <c r="D2" s="25">
+        <v>16</v>
+      </c>
+      <c r="E2" s="25">
+        <v>20</v>
+      </c>
+      <c r="F2" s="25" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" s="25">
+        <v>26</v>
+      </c>
+      <c r="B3" s="25">
+        <v>11</v>
+      </c>
+      <c r="C3" s="25">
+        <v>2024</v>
+      </c>
+      <c r="D3" s="25" t="s">
+        <v>88</v>
+      </c>
+      <c r="E3" s="25" t="s">
+        <v>89</v>
+      </c>
+      <c r="F3" s="25" t="s">
+        <v>91</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <ignoredErrors>
+    <ignoredError sqref="D3" numberStoredAsText="1"/>
+  </ignoredErrors>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC8D5BCD-0BFA-404E-99A9-EC1EBE3315C9}">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="A2" sqref="A2:B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="19.59765625" style="18" customWidth="1"/>
-    <col min="2" max="2" width="28.09765625" style="18" customWidth="1"/>
-    <col min="3" max="16384" width="8.796875" style="18"/>
+    <col min="1" max="1" width="19.59765625" style="14" customWidth="1"/>
+    <col min="2" max="2" width="28.09765625" style="14" customWidth="1"/>
+    <col min="3" max="16384" width="8.796875" style="14"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="18" t="s">
+      <c r="B1" s="14" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:2">
-      <c r="A2" s="18" t="s">
-        <v>59</v>
-      </c>
-      <c r="B2" s="18" t="s">
-        <v>59</v>
+      <c r="A2" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="B2" s="14" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="3" spans="1:2">
-      <c r="A3" s="18" t="s">
-        <v>60</v>
-      </c>
-      <c r="B3" s="18" t="s">
-        <v>60</v>
+      <c r="A3" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="B3" s="14" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="4" spans="1:2">
-      <c r="A4" s="18" t="s">
-        <v>61</v>
-      </c>
-      <c r="B4" s="18" t="s">
-        <v>61</v>
+      <c r="A4" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="B4" s="14" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="5" spans="1:2">
-      <c r="A5" s="18" t="s">
-        <v>62</v>
-      </c>
-      <c r="B5" s="18" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2">
-      <c r="A6" s="18" t="s">
-        <v>63</v>
-      </c>
-      <c r="B6" s="18" t="s">
-        <v>63</v>
+      <c r="A5" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="B5" s="14" t="s">
+        <v>51</v>
       </c>
     </row>
   </sheetData>
@@ -872,104 +1003,105 @@
   <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C14" sqref="A1:XFD1048576"/>
+      <selection activeCell="E14" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="10.09765625" style="1" customWidth="1"/>
-    <col min="2" max="4" width="43.69921875" customWidth="1"/>
-    <col min="5" max="5" width="27" customWidth="1"/>
+    <col min="1" max="1" width="10.09765625" style="18" customWidth="1"/>
+    <col min="2" max="4" width="43.69921875" style="16" customWidth="1"/>
+    <col min="5" max="5" width="27" style="16" customWidth="1"/>
+    <col min="6" max="16384" width="8.796875" style="16"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="D1" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="16" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="27.6">
-      <c r="A2" s="1" t="s">
+    <row r="2" spans="1:5" ht="30">
+      <c r="A2" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="7"/>
-      <c r="D2" s="7"/>
-      <c r="E2" s="5" t="s">
+      <c r="C2" s="20"/>
+      <c r="D2" s="20"/>
+      <c r="E2" s="21" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:5">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="16">
         <v>123</v>
       </c>
-      <c r="E3" s="8" t="s">
+      <c r="E3" s="17" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="27.6">
-      <c r="A4" s="1" t="s">
+    <row r="4" spans="1:5" ht="30">
+      <c r="A4" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="C4" s="10" t="s">
+      <c r="C4" s="22" t="s">
         <v>23</v>
       </c>
-      <c r="D4" s="10"/>
-      <c r="E4" s="5" t="s">
+      <c r="D4" s="22"/>
+      <c r="E4" s="21" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:5">
-      <c r="A5" s="1" t="s">
+      <c r="A5" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="E5" s="8" t="s">
+      <c r="E5" s="17" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="27.6">
-      <c r="A6" s="1" t="s">
+    <row r="6" spans="1:5" ht="30">
+      <c r="A6" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="D6">
+      <c r="D6" s="16">
         <v>123456</v>
       </c>
-      <c r="E6" s="5" t="s">
+      <c r="E6" s="21" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="27.6">
-      <c r="A7" s="1" t="s">
+    <row r="7" spans="1:5" ht="30">
+      <c r="A7" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D7" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="E7" s="5" t="s">
+      <c r="E7" s="21" t="s">
         <v>27</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="6" type="noConversion"/>
+  <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -979,7 +1111,7 @@
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -1010,8 +1142,8 @@
       <c r="B2">
         <v>1</v>
       </c>
-      <c r="C2" s="19" t="s">
-        <v>64</v>
+      <c r="C2" s="15" t="s">
+        <v>52</v>
       </c>
       <c r="D2" s="5" t="s">
         <v>35</v>
@@ -1024,8 +1156,8 @@
       <c r="B3">
         <v>100000</v>
       </c>
-      <c r="C3" s="19" t="s">
-        <v>64</v>
+      <c r="C3" s="15" t="s">
+        <v>52</v>
       </c>
       <c r="D3" s="5" t="s">
         <v>37</v>
@@ -1038,8 +1170,8 @@
       <c r="B4">
         <v>-100</v>
       </c>
-      <c r="C4" s="19" t="s">
-        <v>64</v>
+      <c r="C4" s="15" t="s">
+        <v>52</v>
       </c>
       <c r="D4" s="5" t="s">
         <v>36</v>
@@ -1052,8 +1184,8 @@
       <c r="B5">
         <v>10000000000</v>
       </c>
-      <c r="C5" s="19" t="s">
-        <v>64</v>
+      <c r="C5" s="15" t="s">
+        <v>52</v>
       </c>
       <c r="D5" s="5" t="s">
         <v>38</v>
@@ -1066,13 +1198,13 @@
       <c r="B6">
         <v>10</v>
       </c>
-      <c r="C6" s="19"/>
+      <c r="C6" s="15"/>
       <c r="D6" s="11" t="s">
         <v>40</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="6" type="noConversion"/>
+  <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -1082,7 +1214,7 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.09765625" defaultRowHeight="13.8"/>
@@ -1263,7 +1395,7 @@
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="6" type="noConversion"/>
+  <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -1272,49 +1404,49 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31668794-369D-447D-844B-176076BB7385}">
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="8.796875" style="20"/>
-    <col min="2" max="2" width="83.296875" style="20" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="36.296875" style="20" bestFit="1" customWidth="1"/>
-    <col min="4" max="16384" width="8.796875" style="20"/>
+    <col min="1" max="1" width="8.796875" style="16"/>
+    <col min="2" max="2" width="83.296875" style="16" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="36.296875" style="16" bestFit="1" customWidth="1"/>
+    <col min="4" max="16384" width="8.796875" style="16"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="20" t="s">
-        <v>65</v>
-      </c>
-      <c r="C1" s="20" t="s">
-        <v>69</v>
+      <c r="B1" s="16" t="s">
+        <v>53</v>
+      </c>
+      <c r="C1" s="16" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="2" spans="1:3">
-      <c r="A2" s="20" t="s">
-        <v>70</v>
-      </c>
-      <c r="B2" s="20" t="s">
-        <v>67</v>
-      </c>
-      <c r="C2" s="21" t="s">
-        <v>72</v>
+      <c r="A2" s="16" t="s">
+        <v>58</v>
+      </c>
+      <c r="B2" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="C2" s="17" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="3" spans="1:3">
-      <c r="A3" s="20" t="s">
-        <v>71</v>
-      </c>
-      <c r="B3" s="20" t="s">
-        <v>66</v>
-      </c>
-      <c r="C3" s="21" t="s">
-        <v>68</v>
+      <c r="A3" s="16" t="s">
+        <v>59</v>
+      </c>
+      <c r="B3" s="16" t="s">
+        <v>54</v>
+      </c>
+      <c r="C3" s="17" t="s">
+        <v>56</v>
       </c>
     </row>
   </sheetData>
@@ -1323,187 +1455,224 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FCE42783-E96F-4C8A-AC5E-CFDED4A8E4E5}">
-  <dimension ref="A1:F10"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE4E9F33-4258-4F9D-B7EE-E6E7849C887B}">
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.09765625" defaultRowHeight="13.8"/>
+  <sheetFormatPr defaultColWidth="24.296875" defaultRowHeight="13.8"/>
+  <sheetData>
+    <row r="1" spans="1:2" ht="15">
+      <c r="A1" s="23" t="s">
+        <v>61</v>
+      </c>
+      <c r="B1" s="23" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="30">
+      <c r="A2" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="18" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="30">
+      <c r="A3" s="18" t="s">
+        <v>63</v>
+      </c>
+      <c r="B3" s="18" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="60">
+      <c r="A4" s="18" t="s">
+        <v>65</v>
+      </c>
+      <c r="B4" s="18" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="15">
+      <c r="A5" s="18" t="s">
+        <v>67</v>
+      </c>
+      <c r="B5" s="18" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="15">
+      <c r="B6" s="18" t="s">
+        <v>64</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{09466584-8D5E-4C71-BA21-BCC0B1D9AA4B}">
+  <dimension ref="A1:G6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="18.8984375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="16" style="1" customWidth="1"/>
-    <col min="3" max="3" width="14.3984375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="21.69921875" style="1" customWidth="1"/>
-    <col min="5" max="5" width="22.69921875" style="1" customWidth="1"/>
-    <col min="6" max="6" width="47.296875" style="1" customWidth="1"/>
-    <col min="7" max="16384" width="9.09765625" style="1"/>
+    <col min="1" max="1" width="10.3984375" style="14" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.796875" style="14" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.09765625" style="14" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.8984375" style="14" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.8984375" style="14" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="77.69921875" style="14" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.3984375" style="14" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="8.796875" style="14"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:7">
       <c r="A1" s="14" t="s">
-        <v>48</v>
+        <v>69</v>
       </c>
       <c r="B1" s="14" t="s">
-        <v>49</v>
+        <v>68</v>
       </c>
       <c r="C1" s="14" t="s">
-        <v>50</v>
+        <v>70</v>
       </c>
       <c r="D1" s="14" t="s">
-        <v>51</v>
+        <v>71</v>
       </c>
       <c r="E1" s="14" t="s">
-        <v>52</v>
+        <v>72</v>
       </c>
       <c r="F1" s="14" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" ht="27.6">
-      <c r="A2" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F2" s="17" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6">
-      <c r="A3" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C3" s="1">
-        <v>1000000</v>
-      </c>
-      <c r="F3" s="15" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="4" spans="1:6">
-      <c r="A4" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C4" s="1">
-        <v>-1000000</v>
-      </c>
-      <c r="F4" s="16" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="27.6">
-      <c r="A5" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C5" s="1">
-        <v>10000000</v>
-      </c>
-      <c r="F5" s="17" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6">
-      <c r="A6" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C6" s="1">
-        <v>10000000</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F6" s="16" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6">
-      <c r="A7" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="F7" s="16" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6">
-      <c r="A8" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C8" s="1">
-        <v>1000000</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="F8" s="15" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6">
-      <c r="A9" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C9" s="1">
-        <v>1000000</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E9" s="1">
-        <v>10000</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6">
-      <c r="A10" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C10" s="1">
-        <v>1000000</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E10" s="1">
-        <v>-10000</v>
-      </c>
-      <c r="F10" s="15" t="s">
-        <v>57</v>
+      <c r="G1" s="14" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="24" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="14" t="s">
+        <v>74</v>
+      </c>
+      <c r="D2" s="14">
+        <v>-1</v>
+      </c>
+      <c r="E2" s="14">
+        <v>1</v>
+      </c>
+      <c r="F2" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="G2" s="14" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="24" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="14" t="s">
+        <v>74</v>
+      </c>
+      <c r="D3" s="14">
+        <v>1</v>
+      </c>
+      <c r="E3" s="14">
+        <v>1</v>
+      </c>
+      <c r="F3" s="14" t="s">
+        <v>78</v>
+      </c>
+      <c r="G3" s="14" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" s="24" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" s="14" t="s">
+        <v>74</v>
+      </c>
+      <c r="D4" s="14">
+        <v>1</v>
+      </c>
+      <c r="E4" s="14">
+        <v>-1</v>
+      </c>
+      <c r="F4" s="14" t="s">
+        <v>80</v>
+      </c>
+      <c r="G4" s="14" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="B5" s="24" t="s">
+        <v>2</v>
+      </c>
+      <c r="C5" s="14" t="s">
+        <v>74</v>
+      </c>
+      <c r="D5" s="14">
+        <v>1</v>
+      </c>
+      <c r="E5" s="14">
+        <v>1</v>
+      </c>
+      <c r="F5" s="14" t="s">
+        <v>78</v>
+      </c>
+      <c r="G5" s="14" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="A6" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="B6" s="24" t="s">
+        <v>2</v>
+      </c>
+      <c r="C6" s="14" t="s">
+        <v>74</v>
+      </c>
+      <c r="D6" s="14">
+        <v>1</v>
+      </c>
+      <c r="E6" s="14">
+        <v>1</v>
+      </c>
+      <c r="F6" s="14" t="s">
+        <v>78</v>
+      </c>
+      <c r="G6" s="14" t="s">
+        <v>82</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>